<commit_message>
Prevent storekeepers from directly issuing materials without approval
Removes direct material issuance functionality from storesperson view and implements issuance request workflow in `routes.py` and `storesperson.html`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: c4bceaa7-b495-48fa-9d9c-e86f62df6227
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4e599e1f-39b3-4c73-bffa-3b0c52532fec/de9b845e-ffce-413f-8425-fad6fe3b63c8.jpg
</commit_message>
<xml_diff>
--- a/data/construction_materials.xlsx
+++ b/data/construction_materials.xlsx
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -465,12 +465,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-07-10 11:05:50</t>
+          <t>2025-07-10 12:19:24</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Site Engineer</t>
+          <t>storesperson</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,39 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-07-10 12:19:24</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>White Tiles</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>boxes</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>storesperson</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>To tiler</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add initial project documentation and inventory tracking sample data
Include a detailed project proposal and a sample construction material data file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: c4bceaa7-b495-48fa-9d9c-e86f62df6227
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/4e599e1f-39b3-4c73-bffa-3b0c52532fec/d6d82031-0339-431c-a64e-6caa704296c1.jpg
</commit_message>
<xml_diff>
--- a/data/construction_materials.xlsx
+++ b/data/construction_materials.xlsx
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -465,12 +465,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-07-10 12:19:24</t>
+          <t>2025-07-10 12:45:18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>storesperson</t>
+          <t>engineer</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -490,12 +490,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-07-10 11:05:50</t>
+          <t>2025-07-10 12:45:18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Site Engineer</t>
+          <t>engineer</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,6 +588,72 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-07-10 12:45:18</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>White Tiles</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>boxes</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>engineer</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Batch BTH-20250710-624B - Authorized by engineer</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-07-10 12:45:18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Cement (50 Kgs)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>bags</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>engineer</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Batch BTH-20250710-624B - Authorized by engineer</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>